<commit_message>
Completed pagination and limit
</commit_message>
<xml_diff>
--- a/backend/src/data/files/data.xlsx
+++ b/backend/src/data/files/data.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvin\Downloads\projects\MIS-Legal-Firm\backend\src\data\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01921373-E47D-45D7-8B2A-27314AEDB3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A47580-03FF-4A3D-9AC2-43F8A2D3E72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="COMP" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>

</xml_diff>